<commit_message>
Initial Fan Duct Commit
</commit_message>
<xml_diff>
--- a/Part File Library/Source Files/Chrisousel/BOM.xlsx
+++ b/Part File Library/Source Files/Chrisousel/BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>BOM for Chrisousel</t>
   </si>
@@ -85,13 +85,49 @@
   </si>
   <si>
     <t>Likely to be replaced</t>
+  </si>
+  <si>
+    <t>Fan Duct</t>
+  </si>
+  <si>
+    <t>M3x30 Male Standoff</t>
+  </si>
+  <si>
+    <t>M3x40 Female Standoff</t>
+  </si>
+  <si>
+    <t>M4x14 Cap Head Screw</t>
+  </si>
+  <si>
+    <t>6020 Fan</t>
+  </si>
+  <si>
+    <t>High CFM</t>
+  </si>
+  <si>
+    <t>PTC Heater 12x7cm 260C</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/1005003758412972.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YEKMLCO Soldering Plate with Cord </t>
+  </si>
+  <si>
+    <t>SSR</t>
+  </si>
+  <si>
+    <t>10A for 120v service, 5a for 220v service</t>
+  </si>
+  <si>
+    <t>Thermal Fuse 105C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +139,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -125,14 +169,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -432,16 +479,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -586,7 +633,86 @@
         <v>20</v>
       </c>
     </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E23" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>